<commit_message>
updata daya tampung dan lulusan
</commit_message>
<xml_diff>
--- a/static/dt.xlsx
+++ b/static/dt.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\# REGISTRASI DAN STATISTIK\Website\202101\202101\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C7EC25F-7D72-476C-BC05-6C833E1EDFF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F75B7CC-C03A-470E-8812-5EE126D08C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Program Studi</t>
   </si>
@@ -31,9 +32,6 @@
     <t>SBMPTN</t>
   </si>
   <si>
-    <t>SMMPTN</t>
-  </si>
-  <si>
     <t>TA</t>
   </si>
   <si>
@@ -215,13 +213,19 @@
   </si>
   <si>
     <t>Pendidikan (S3)</t>
+  </si>
+  <si>
+    <t>MANDIRI</t>
+  </si>
+  <si>
+    <t>Keperawatan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +360,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -654,7 +666,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -697,11 +709,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -739,6 +752,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{51E53669-B3EA-4478-AFEB-812E9182AB60}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1054,12 +1068,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1072,15 +1091,15 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>120</v>
@@ -1097,7 +1116,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>36</v>
@@ -1114,7 +1133,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>36</v>
@@ -1131,7 +1150,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>36</v>
@@ -1148,7 +1167,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>36</v>
@@ -1165,7 +1184,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>36</v>
@@ -1182,7 +1201,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>36</v>
@@ -1199,7 +1218,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>24</v>
@@ -1216,7 +1235,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>24</v>
@@ -1233,7 +1252,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -1250,7 +1269,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>24</v>
@@ -1267,7 +1286,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>24</v>
@@ -1284,7 +1303,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>24</v>
@@ -1301,7 +1320,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>24</v>
@@ -1318,7 +1337,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>24</v>
@@ -1335,7 +1354,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>24</v>
@@ -1352,7 +1371,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>24</v>
@@ -1369,7 +1388,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>24</v>
@@ -1386,7 +1405,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>24</v>
@@ -1403,7 +1422,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -1420,7 +1439,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>36</v>
@@ -1437,7 +1456,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>36</v>
@@ -1454,7 +1473,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>36</v>
@@ -1471,7 +1490,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>36</v>
@@ -1488,7 +1507,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>36</v>
@@ -1505,7 +1524,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>24</v>
@@ -1522,7 +1541,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>60</v>
@@ -1539,7 +1558,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>60</v>
@@ -1556,7 +1575,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>36</v>
@@ -1573,7 +1592,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>36</v>
@@ -1590,7 +1609,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>12</v>
@@ -1607,7 +1626,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>42</v>
@@ -1624,7 +1643,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>42</v>
@@ -1641,7 +1660,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>24</v>
@@ -1658,7 +1677,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>12</v>
@@ -1675,7 +1694,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>48</v>
@@ -1692,7 +1711,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>60</v>
@@ -1709,7 +1728,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>36</v>
@@ -1726,16 +1745,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="C40">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="D40">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E40">
         <v>2020</v>
@@ -1743,16 +1762,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C41">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D41">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E41">
         <v>2020</v>
@@ -1760,13 +1779,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C42">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D42">
         <v>36</v>
@@ -1777,16 +1796,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B43">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C43">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D43">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E43">
         <v>2020</v>
@@ -1794,16 +1813,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C44">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D44">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E44">
         <v>2020</v>
@@ -1811,16 +1830,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C45">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D45">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E45">
         <v>2020</v>
@@ -1828,16 +1847,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C46">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D46">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E46">
         <v>2020</v>
@@ -1845,13 +1864,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C47">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D47">
         <v>24</v>
@@ -1862,13 +1881,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C48">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D48">
         <v>24</v>
@@ -1879,16 +1898,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B49">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C49">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D49">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E49">
         <v>2020</v>
@@ -1896,13 +1915,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50">
         <v>16</v>
       </c>
-      <c r="B50">
-        <v>24</v>
-      </c>
       <c r="C50">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D50">
         <v>24</v>
@@ -1913,13 +1932,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D51">
         <v>24</v>
@@ -1930,13 +1949,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D52">
         <v>24</v>
@@ -1947,16 +1966,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B53">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D53">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E53">
         <v>2020</v>
@@ -1964,13 +1983,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54">
+        <v>16</v>
+      </c>
+      <c r="C54">
         <v>48</v>
-      </c>
-      <c r="B54">
-        <v>24</v>
-      </c>
-      <c r="C54">
-        <v>32</v>
       </c>
       <c r="D54">
         <v>24</v>
@@ -1981,13 +2000,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C55">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D55">
         <v>24</v>
@@ -1998,13 +2017,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D56">
         <v>24</v>
@@ -2015,13 +2034,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C57">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D57">
         <v>24</v>
@@ -2032,13 +2051,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B58">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C58">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D58">
         <v>24</v>
@@ -2049,13 +2068,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C59">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D59">
         <v>36</v>
@@ -2066,16 +2085,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C60">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D60">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E60">
         <v>2020</v>
@@ -2083,13 +2102,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B61">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C61">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D61">
         <v>36</v>
@@ -2100,16 +2119,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B62">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C62">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D62">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E62">
         <v>2020</v>
@@ -2117,13 +2136,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B63">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C63">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D63">
         <v>36</v>
@@ -2134,16 +2153,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C64">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D64">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E64">
         <v>2020</v>
@@ -2151,16 +2170,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B65">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C65">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D65">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E65">
         <v>2020</v>
@@ -2168,13 +2187,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B66">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C66">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="D66">
         <v>60</v>
@@ -2185,16 +2204,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B67">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C67">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D67">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E67">
         <v>2020</v>
@@ -2202,13 +2221,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C68">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D68">
         <v>36</v>
@@ -2219,16 +2238,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B69">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C69">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="D69">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E69">
         <v>2020</v>
@@ -2236,16 +2255,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C70">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="D70">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E70">
         <v>2020</v>
@@ -2253,16 +2272,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B71">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C71">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="D71">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E71">
         <v>2020</v>
@@ -2270,16 +2289,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B72">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C72">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D72">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E72">
         <v>2020</v>
@@ -2287,16 +2306,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B73">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C73">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D73">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E73">
         <v>2020</v>
@@ -2304,16 +2323,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B74">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C74">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="D74">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E74">
         <v>2020</v>
@@ -2321,16 +2340,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B75">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C75">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D75">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="E75">
         <v>2020</v>
@@ -2338,13 +2357,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B76">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C76">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D76">
         <v>15</v>
@@ -2355,16 +2374,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B77">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C77">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D77">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E77">
         <v>2020</v>
@@ -2372,13 +2391,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B78">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C78">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D78">
         <v>12</v>
@@ -2389,10 +2408,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>54</v>
+        <v>65</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="E79">
         <v>2020</v>
@@ -2400,10 +2425,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E80">
         <v>2020</v>
@@ -2411,10 +2442,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
       </c>
       <c r="D81">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E81">
         <v>2020</v>
@@ -2422,10 +2459,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E82">
         <v>2020</v>
@@ -2433,10 +2476,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E83">
         <v>2020</v>
@@ -2444,10 +2493,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>7</v>
+        <v>57</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="E84">
         <v>2020</v>
@@ -2455,10 +2510,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>59</v>
+        <v>6</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E85">
         <v>2020</v>
@@ -2466,10 +2527,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>5</v>
+        <v>58</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E86">
         <v>2020</v>
@@ -2477,10 +2544,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>60</v>
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E87">
         <v>2020</v>
@@ -2488,7 +2561,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
       </c>
       <c r="D88">
         <v>40</v>
@@ -2499,10 +2578,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E89">
         <v>2020</v>
@@ -2510,10 +2595,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>8</v>
+        <v>61</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E90">
         <v>2020</v>
@@ -2521,7 +2612,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
       </c>
       <c r="D91">
         <v>40</v>
@@ -2532,7 +2629,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>8</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
       </c>
       <c r="D92">
         <v>40</v>
@@ -2543,7 +2646,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>29</v>
+        <v>62</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
       </c>
       <c r="D93">
         <v>40</v>
@@ -2554,7 +2663,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
       </c>
       <c r="D94">
         <v>40</v>
@@ -2565,12 +2680,35 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>64</v>
+        <v>40</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
       </c>
       <c r="D95">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E95">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>63</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>25</v>
+      </c>
+      <c r="E96">
         <v>2020</v>
       </c>
     </row>

</xml_diff>